<commit_message>
update xuat excel phieu muon va excel thong ke
</commit_message>
<xml_diff>
--- a/QuanLyThuVienHUFI/Form_QuanLyThuVien/bin/Debug/DanhSachPhieuMuonTreHanChuaTra.xlsx
+++ b/QuanLyThuVienHUFI/Form_QuanLyThuVien/bin/Debug/DanhSachPhieuMuonTreHanChuaTra.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>TRƯỜNG ĐẠI HỌC CÔNG NGHIỆP THỰC PHẨM TP.HCM</t>
   </si>
@@ -44,13 +44,13 @@
     <t>Họ và tên người in:</t>
   </si>
   <si>
-    <t>Nguyễn Văn A</t>
+    <t>Nguyễn Nhật Lâm</t>
   </si>
   <si>
     <t>Mã số thẻ người in:</t>
   </si>
   <si>
-    <t>10000003</t>
+    <t>10000002</t>
   </si>
   <si>
     <t>Mã phiếu mượn</t>
@@ -77,28 +77,16 @@
     <t>2001170373</t>
   </si>
   <si>
-    <t>Nguyễn Nhật Lâm</t>
-  </si>
-  <si>
     <t>26/01/2019</t>
   </si>
   <si>
-    <t>716</t>
+    <t>723</t>
   </si>
   <si>
     <t>4</t>
   </si>
   <si>
     <t>2001170018</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>2033207524</t>
-  </si>
-  <si>
-    <t>2</t>
   </si>
   <si>
     <t>6</t>
@@ -650,117 +638,101 @@
         <v>15</v>
       </c>
       <c r="D13" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13" s="4" t="s">
         <v>16</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>17</v>
       </c>
       <c r="F13" s="4" t="s">
         <v>14</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" ht="25.8" customHeight="1">
       <c r="B14" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="4" t="s">
-        <v>20</v>
-      </c>
       <c r="D14" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E14" s="4" t="s">
         <v>16</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>17</v>
       </c>
       <c r="F14" s="4" t="s">
         <v>14</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" ht="24" customHeight="1">
       <c r="B15" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="D15" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F15" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D15" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E15" s="4" t="s">
+      <c r="G15" s="4" t="s">
         <v>17</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="16">
       <c r="B16" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D16" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E16" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="F16" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G16" s="4" t="s">
         <v>17</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="17" ht="15.6">
       <c r="B17" s="4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D17" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E17" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E17" s="4" t="s">
+      <c r="F17" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G17" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F17" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="G17" s="4" t="s">
-        <v>18</v>
-      </c>
     </row>
     <row r="18" ht="15.6">
-      <c r="B18" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>18</v>
-      </c>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
     </row>
     <row r="19" ht="14.4" customHeight="1">
       <c r="D19" s="6"/>

</xml_diff>